<commit_message>
add preliminary analysis file and finalize curve fits, merge with pre canopy closure data file
</commit_message>
<xml_diff>
--- a/licor_data/licor_log_files/licor_log_file_blank.xlsx
+++ b/licor_data/licor_log_files/licor_log_file_blank.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/2023_field_campaign/licor_log_files/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/eaperkowski/git/trillium_trail/licor_data/licor_log_files/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3DE01A36-2308-D44C-B633-7C79939D2804}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09DD0CAD-A91C-0442-962D-DCA4D7E3CAEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="15620" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
+    <workbookView xWindow="1660" yWindow="500" windowWidth="28800" windowHeight="15620" xr2:uid="{E2101264-4A8C-BA4C-A9EF-E5EFE562CDE8}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="96" uniqueCount="22">
   <si>
     <t>LICOR CHAMBER CONDITIONS</t>
   </si>
@@ -94,6 +94,15 @@
   </si>
   <si>
     <t>420 (before curve)</t>
+  </si>
+  <si>
+    <t>MAI</t>
+  </si>
+  <si>
+    <t>NO TIME</t>
+  </si>
+  <si>
+    <t>STARTED TOO SOON; MAY BE BAD CURVE</t>
   </si>
 </sst>
 </file>
@@ -186,7 +195,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -208,6 +217,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="20" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -527,8 +539,8 @@
   </sheetPr>
   <dimension ref="A1:H26"/>
   <sheetViews>
-    <sheetView tabSelected="1" view="pageLayout" topLeftCell="A19" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B4" sqref="A2:B4"/>
+    <sheetView tabSelected="1" view="pageLayout" zoomScaleNormal="86" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -566,8 +578,12 @@
       </c>
     </row>
     <row r="2" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A2" s="6"/>
-      <c r="B2" s="6"/>
+      <c r="A2" s="6">
+        <v>2616</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C2" s="5" t="s">
         <v>5</v>
       </c>
@@ -580,12 +596,18 @@
       <c r="F2" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G2" s="7"/>
+      <c r="G2" s="11">
+        <v>0.46527777777777773</v>
+      </c>
       <c r="H2" s="7"/>
     </row>
     <row r="3" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A3" s="6"/>
-      <c r="B3" s="6"/>
+      <c r="A3" s="6">
+        <v>1476</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C3" s="5" t="s">
         <v>5</v>
       </c>
@@ -598,12 +620,18 @@
       <c r="F3" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G3" s="7"/>
+      <c r="G3" s="11">
+        <v>0.52500000000000002</v>
+      </c>
       <c r="H3" s="7"/>
     </row>
     <row r="4" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A4" s="6"/>
-      <c r="B4" s="6"/>
+      <c r="A4" s="6">
+        <v>4781</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C4" s="5" t="s">
         <v>5</v>
       </c>
@@ -616,12 +644,20 @@
       <c r="F4" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G4" s="7"/>
-      <c r="H4" s="7"/>
+      <c r="G4" s="11">
+        <v>0.53749999999999998</v>
+      </c>
+      <c r="H4" s="7" t="s">
+        <v>21</v>
+      </c>
     </row>
     <row r="5" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A5" s="6"/>
-      <c r="B5" s="6"/>
+      <c r="A5" s="6">
+        <v>5052</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>19</v>
+      </c>
       <c r="C5" s="5" t="s">
         <v>5</v>
       </c>
@@ -634,7 +670,9 @@
       <c r="F5" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="7"/>
+      <c r="G5" s="7" t="s">
+        <v>20</v>
+      </c>
       <c r="H5" s="7"/>
     </row>
     <row r="6" spans="1:8" ht="60" customHeight="1" x14ac:dyDescent="0.45">
@@ -971,9 +1009,9 @@
   <pageSetup scale="48" orientation="portrait" horizontalDpi="0" verticalDpi="0" copies="50"/>
   <headerFooter alignWithMargins="0">
     <oddHeader>&amp;L&amp;"Calibri (Body),Regular"&amp;24
-Date: __________________&amp;C&amp;"Calibri (Body),Regular"&amp;18Machine (circle):
-&amp;24Ozz   Gib    Alb    Stan    Yat&amp;R&amp;"Calibri (Body),Regular"&amp;20
-Licor Enthusiast: ____________________</oddHeader>
+Date: JUNE 15, 2023&amp;C&amp;"Calibri (Body),Regular"&amp;18Machine (circle):
+&amp;24Ozz   Gib    Alb    Stan    &amp;"Calibri (Body),Bold"Yat&amp;R&amp;"Calibri (Body),Regular"&amp;20
+Licor Enthusiast: EVAN PERKOWSKI</oddHeader>
     <oddFooter>&amp;L&amp;"Calibri (Body),Regular"&amp;20Weather notes:</oddFooter>
   </headerFooter>
 </worksheet>

</xml_diff>